<commit_message>
[Tech|Misc] Sync 25/12/10 - 01:25
- 코드 클린업 하기전 백업 커밋
</commit_message>
<xml_diff>
--- a/AssetLibrary/Character/DvMannequin/Animation Naming Convention.xlsx
+++ b/AssetLibrary/Character/DvMannequin/Animation Naming Convention.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wkspace\Divergent\main\Data\AssetLibrary\Character\DvMannequin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C051ED-30B8-4FF9-BA79-8EE79F6A8D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E60870-9E7F-44ED-97FD-47A5092EDEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="600" windowWidth="14400" windowHeight="15600" xr2:uid="{C20D2E47-0230-46BF-AA16-4B353B6511BC}"/>
+    <workbookView minimized="1" xWindow="3828" yWindow="6192" windowWidth="23040" windowHeight="12204" xr2:uid="{C20D2E47-0230-46BF-AA16-4B353B6511BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="83">
   <si>
     <t>Armed State</t>
   </si>
@@ -1213,6 +1213,18 @@
   </si>
   <si>
     <t>Sprinting</t>
+  </si>
+  <si>
+    <t>ItemHeldContext</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RifleArmed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1697,7 +1709,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1803,9 +1815,69 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1814,84 +1886,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2227,15 +2221,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5ECE54-6C7A-42C1-A04D-518AD5743354}">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G51" sqref="A24:G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.8984375" customWidth="1"/>
     <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
@@ -2245,35 +2239,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:13" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:13" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>1</v>
@@ -2350,7 +2344,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="str" cm="1">
+        <f t="array" ref="G6">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A6:E6, "-", ""))</f>
+        <v/>
+      </c>
       <c r="H6" s="30"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -2362,184 +2359,146 @@
         <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="str" cm="1">
         <f t="array" ref="G7">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A7:E7, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_Forward</v>
-      </c>
-      <c r="H7" s="32"/>
+        <v>AS_RifleArmed_Standing_idle</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A8" s="29"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="str" cm="1">
         <f t="array" ref="G8">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A8:E8, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_ForwardLeft</v>
-      </c>
-      <c r="H8" s="32"/>
+        <v/>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A9" s="29"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1" t="str" cm="1">
-        <f t="array" ref="G9">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A9:E9, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_ForwardRight</v>
-      </c>
-      <c r="H9" s="32"/>
+      <c r="G9" s="1" t="e" cm="1">
+        <f t="array" ref="G9">B3It=_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A9:E9, "-", ""))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="29"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="str" cm="1">
         <f t="array" ref="G10">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A10:E10, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_Backward</v>
-      </c>
-      <c r="H10" s="32"/>
+        <v/>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A11" s="29"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="str" cm="1">
         <f t="array" ref="G11">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A11:E11, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_BackwardLeft</v>
-      </c>
-      <c r="H11" s="32"/>
+        <v/>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A12" s="29"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="str" cm="1">
         <f t="array" ref="G12">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A12:E12, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_BackwardRight</v>
-      </c>
-      <c r="H12" s="32"/>
+        <v/>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A13" s="29"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="str" cm="1">
         <f t="array" ref="G13">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A13:E13, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_Left</v>
-      </c>
-      <c r="H13" s="32"/>
+        <v/>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A14" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A14" s="29"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="str" cm="1">
         <f t="array" ref="G14">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A14:E14, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Walking_Right</v>
-      </c>
-      <c r="H14" s="32"/>
+        <v/>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="29"/>
@@ -2548,22 +2507,28 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="str" cm="1">
+        <f t="array" ref="G15">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A15:E15, "-", ""))</f>
+        <v/>
+      </c>
       <c r="H15" s="30"/>
       <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
@@ -2571,23 +2536,22 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A16:E16, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_Forward</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="J16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_Forward</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>30</v>
@@ -2595,22 +2559,22 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A17:E17, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_ForwardLeft</v>
-      </c>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_ForwardLeft</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>31</v>
@@ -2618,22 +2582,22 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="str" cm="1">
         <f t="array" ref="G18">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A18:E18, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_ForwardRight</v>
-      </c>
-      <c r="H18" s="30"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_ForwardRight</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
@@ -2641,22 +2605,22 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="str" cm="1">
         <f t="array" ref="G19">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A19:E19, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_Backward</v>
-      </c>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_Backward</v>
+      </c>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
@@ -2664,22 +2628,22 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A20:E20, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_BackwardLeft</v>
-      </c>
-      <c r="H20" s="30"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_BackwardLeft</v>
+      </c>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>29</v>
@@ -2687,22 +2651,22 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A21:E21, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_BackwardRight</v>
-      </c>
-      <c r="H21" s="30"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_BackwardRight</v>
+      </c>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>32</v>
@@ -2710,22 +2674,22 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="str" cm="1">
         <f t="array" ref="G22">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A22:E22, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_Left</v>
-      </c>
-      <c r="H22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_Left</v>
+      </c>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>33</v>
@@ -2733,24 +2697,22 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A23:E23, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Running_Right</v>
-      </c>
-      <c r="H23" s="30"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Walking_Right</v>
+      </c>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="29"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1" t="str" cm="1">
-        <f t="array" ref="G24">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A24:E24, "-", ""))</f>
-        <v/>
-      </c>
+      <c r="G24" s="1"/>
       <c r="H24" s="30"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J24" s="24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="29" t="s">
         <v>66</v>
       </c>
@@ -2761,7 +2723,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>9</v>
@@ -2769,305 +2731,313 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A25:E25, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Sprinting_Forward</v>
+        <v>AS_UnArmed_Standing_Running_Forward</v>
       </c>
       <c r="H25" s="30"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" s="29"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="J25" s="24"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A26:E26, "-", ""))</f>
-        <v/>
-      </c>
-      <c r="H26" s="32"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Running_ForwardLeft</v>
+      </c>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E27" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="str" cm="1">
         <f t="array" ref="G27">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A27:E27, "-", ""))</f>
-        <v>BS_UnArmed_Standing_Moving</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28" s="29"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="E28" s="1"/>
+        <v>AS_UnArmed_Standing_Running_ForwardRight</v>
+      </c>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="33"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G28" s="1" t="str" cm="1">
+        <f t="array" ref="G28">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A28:E28, "-", ""))</f>
+        <v>AS_UnArmed_Standing_Running_Backward</v>
+      </c>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="58" t="s">
+      <c r="B29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="45"/>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1" t="str" cm="1">
         <f t="array" ref="G29">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A29:E29, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Turning_Left</v>
-      </c>
-      <c r="H29" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Running_BackwardLeft</v>
+      </c>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="58" t="s">
+      <c r="B30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="45"/>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1" t="str" cm="1">
         <f t="array" ref="G30">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A30:E30, "-", ""))</f>
-        <v>AS_UnArmed_Standing_Turning_Right</v>
-      </c>
-      <c r="H30" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A31" s="31"/>
+        <v>AS_UnArmed_Standing_Running_BackwardRight</v>
+      </c>
+      <c r="H30" s="30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1" t="str" cm="1">
         <f t="array" ref="G31">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A31:E31, "-", ""))</f>
-        <v/>
-      </c>
-      <c r="H31" s="32"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+        <v>AS_UnArmed_Standing_Running_Left</v>
+      </c>
+      <c r="H31" s="30"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="str" cm="1">
         <f t="array" ref="G32">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A32:E32, "-", ""))</f>
-        <v>AP_UnArmed_Crouching</v>
-      </c>
-      <c r="H32" s="30" t="s">
-        <v>26</v>
-      </c>
+        <v>AS_UnArmed_Standing_Running_Right</v>
+      </c>
+      <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A33" s="29"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="str" cm="1">
         <f t="array" ref="G33">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A33:E33, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Idle</v>
-      </c>
-      <c r="H33" s="32"/>
+        <v/>
+      </c>
+      <c r="H33" s="30"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A34" s="29"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="A34" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="32"/>
+      <c r="G34" s="1" t="str" cm="1">
+        <f t="array" ref="G34">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A34:E34, "-", ""))</f>
+        <v>AS_UnArmed_Standing_Sprinting_Forward</v>
+      </c>
+      <c r="H34" s="30"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A35" s="29"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="str" cm="1">
         <f t="array" ref="G35">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A35:E35, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_Forward</v>
+        <v/>
       </c>
       <c r="H35" s="32"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="str" cm="1">
         <f t="array" ref="G36">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A36:E36, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_ForwardLeft</v>
-      </c>
-      <c r="H36" s="32"/>
+        <v>BS_UnArmed_Standing_Moving</v>
+      </c>
+      <c r="H36" s="33" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A37" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A37" s="29"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1" t="str" cm="1">
-        <f t="array" ref="G37">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A37:E37, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_ForwardRight</v>
-      </c>
-      <c r="H37" s="32"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="33"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>11</v>
+      <c r="B38" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>5</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="str" cm="1">
         <f t="array" ref="G38">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A38:E38, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_Backward</v>
-      </c>
-      <c r="H38" s="32"/>
+        <v>AS_UnArmed_Standing_Turning_Left</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>10</v>
+      <c r="B39" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>71</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="str" cm="1">
         <f t="array" ref="G39">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A39:E39, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_BackwardLeft</v>
-      </c>
-      <c r="H39" s="32"/>
+        <v>AS_UnArmed_Standing_Turning_Right</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A40" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="1"/>
+      <c r="A40" s="31"/>
       <c r="G40" s="1" t="str" cm="1">
         <f t="array" ref="G40">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A40:E40, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_BackwardRight</v>
+        <v/>
       </c>
       <c r="H40" s="32"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="29" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>4</v>
@@ -3075,18 +3045,16 @@
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="str" cm="1">
         <f t="array" ref="G41">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A41:E41, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_Left</v>
-      </c>
-      <c r="H41" s="32"/>
+        <v>AP_UnArmed_Crouching</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="29" t="s">
@@ -3098,16 +3066,14 @@
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="str" cm="1">
         <f t="array" ref="G42">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A42:E42, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Walking_Right</v>
+        <v>AS_UnArmed_Crouching_Idle</v>
       </c>
       <c r="H42" s="32"/>
     </row>
@@ -3132,7 +3098,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>9</v>
@@ -3140,7 +3106,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="str" cm="1">
         <f t="array" ref="G44">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A44:E44, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_Forward</v>
+        <v>AS_UnArmed_Crouching_Walking_Forward</v>
       </c>
       <c r="H44" s="32"/>
     </row>
@@ -3155,7 +3121,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>30</v>
@@ -3163,7 +3129,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="str" cm="1">
         <f t="array" ref="G45">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A45:E45, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_ForwardLeft</v>
+        <v>AS_UnArmed_Crouching_Walking_ForwardLeft</v>
       </c>
       <c r="H45" s="32"/>
     </row>
@@ -3178,7 +3144,7 @@
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>31</v>
@@ -3186,7 +3152,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="str" cm="1">
         <f t="array" ref="G46">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A46:E46, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_ForwardRight</v>
+        <v>AS_UnArmed_Crouching_Walking_ForwardRight</v>
       </c>
       <c r="H46" s="32"/>
     </row>
@@ -3201,7 +3167,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>8</v>
@@ -3209,7 +3175,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="str" cm="1">
         <f t="array" ref="G47">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A47:E47, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_Backward</v>
+        <v>AS_UnArmed_Crouching_Walking_Backward</v>
       </c>
       <c r="H47" s="32"/>
     </row>
@@ -3224,7 +3190,7 @@
         <v>11</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>28</v>
@@ -3232,7 +3198,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="str" cm="1">
         <f t="array" ref="G48">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A48:E48, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_BackwardLeft</v>
+        <v>AS_UnArmed_Crouching_Walking_BackwardLeft</v>
       </c>
       <c r="H48" s="32"/>
     </row>
@@ -3247,7 +3213,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>29</v>
@@ -3255,7 +3221,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="str" cm="1">
         <f t="array" ref="G49">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A49:E49, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_BackwardRight</v>
+        <v>AS_UnArmed_Crouching_Walking_BackwardRight</v>
       </c>
       <c r="H49" s="32"/>
     </row>
@@ -3270,7 +3236,7 @@
         <v>11</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>32</v>
@@ -3278,7 +3244,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="str" cm="1">
         <f t="array" ref="G50">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A50:E50, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_Left</v>
+        <v>AS_UnArmed_Crouching_Walking_Left</v>
       </c>
       <c r="H50" s="32"/>
     </row>
@@ -3293,7 +3259,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>33</v>
@@ -3301,7 +3267,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="str" cm="1">
         <f t="array" ref="G51">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A51:E51, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Running_Right</v>
+        <v>AS_UnArmed_Crouching_Walking_Right</v>
       </c>
       <c r="H51" s="32"/>
     </row>
@@ -3320,13 +3286,13 @@
         <v>66</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>9</v>
@@ -3334,481 +3300,675 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="str" cm="1">
         <f t="array" ref="G53">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A53:E53, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Sprinting_Forward</v>
-      </c>
-      <c r="H53" s="30"/>
+        <v>AS_UnArmed_Crouching_Running_Forward</v>
+      </c>
+      <c r="H53" s="32"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A54" s="31"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="A54" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="str" cm="1">
         <f t="array" ref="G54">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A54:E54, "-", ""))</f>
-        <v/>
+        <v>AS_UnArmed_Crouching_Running_ForwardLeft</v>
       </c>
       <c r="H54" s="32"/>
     </row>
-    <row r="55" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="58" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A55" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="59"/>
-      <c r="E55" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58" t="str" cm="1">
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1" t="str" cm="1">
         <f t="array" ref="G55">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A55:E55, "-", ""))</f>
-        <v>BS_UnArmed_Crouching_Moving</v>
-      </c>
-      <c r="H55" s="60" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="44"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61" t="str" cm="1">
+        <v>AS_UnArmed_Crouching_Running_ForwardRight</v>
+      </c>
+      <c r="H55" s="32"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A56" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1" t="str" cm="1">
         <f t="array" ref="G56">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A56:E56, "-", ""))</f>
-        <v/>
-      </c>
-      <c r="H56" s="46"/>
+        <v>AS_UnArmed_Crouching_Running_Backward</v>
+      </c>
+      <c r="H56" s="32"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="45" t="s">
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45" t="str" cm="1">
+      <c r="D57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="str" cm="1">
         <f t="array" ref="G57">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A57:E57, "-", ""))</f>
-        <v>AS_UnArmed_Crouching_Turning_Left</v>
-      </c>
-      <c r="H57" s="46" t="s">
-        <v>78</v>
-      </c>
+        <v>AS_UnArmed_Crouching_Running_BackwardLeft</v>
+      </c>
+      <c r="H57" s="32"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="45" t="s">
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="47" t="s">
+      <c r="D58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="str" cm="1">
+        <f t="array" ref="G58">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A58:E58, "-", ""))</f>
+        <v>AS_UnArmed_Crouching_Running_BackwardRight</v>
+      </c>
+      <c r="H58" s="32"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A59" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="str" cm="1">
+        <f t="array" ref="G59">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A59:E59, "-", ""))</f>
+        <v>AS_UnArmed_Crouching_Running_Left</v>
+      </c>
+      <c r="H59" s="32"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A60" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1" t="str" cm="1">
+        <f t="array" ref="G60">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A60:E60, "-", ""))</f>
+        <v>AS_UnArmed_Crouching_Running_Right</v>
+      </c>
+      <c r="H60" s="32"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A61" s="29"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="32"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A62" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1" t="str" cm="1">
+        <f t="array" ref="G62">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A62:E62, "-", ""))</f>
+        <v>AS_UnArmed_Crouching_Sprinting_Forward</v>
+      </c>
+      <c r="H62" s="30"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A63" s="31"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1" t="str" cm="1">
+        <f t="array" ref="G63">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A63:E63, "-", ""))</f>
+        <v/>
+      </c>
+      <c r="H63" s="32"/>
+    </row>
+    <row r="64" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="46"/>
+      <c r="E64" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45" t="str" cm="1">
+        <f t="array" ref="G64">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A64:E64, "-", ""))</f>
+        <v>BS_UnArmed_Crouching_Moving</v>
+      </c>
+      <c r="H64" s="47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="24"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48" t="str" cm="1">
+        <f t="array" ref="G65">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A65:E65, "-", ""))</f>
+        <v/>
+      </c>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A66" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E58" s="45" t="s">
+      <c r="E66" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1" t="str" cm="1">
+        <f t="array" ref="G66">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A66:E66, "-", ""))</f>
+        <v>AS_UnArmed_Crouching_Turning_Left</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A67" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45" t="str" cm="1">
-        <f t="array" ref="G58">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A58:E58, "-", ""))</f>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1" t="str" cm="1">
+        <f t="array" ref="G67">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A67:E67, "-", ""))</f>
         <v>AS_UnArmed_Crouching_Turning_Right</v>
       </c>
-      <c r="H58" s="46" t="s">
+      <c r="H67" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58" t="str" cm="1">
-        <f t="array" ref="G59">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A59:E59, "-", ""))</f>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B68" s="45"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45" t="str" cm="1">
+        <f t="array" ref="G68">_xlfn.TEXTJOIN("_", TRUE, SUBSTITUTE(A68:E68, "-", ""))</f>
         <v/>
       </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="43" t="s">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
-    </row>
-    <row r="62" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="53" t="s">
+      <c r="B70" s="56"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="56"/>
+      <c r="H70" s="56"/>
+    </row>
+    <row r="71" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="54" t="s">
+      <c r="B71" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="55" t="s">
+      <c r="C71" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="56" t="s">
+      <c r="D71" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E71" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="55" t="s">
+      <c r="F71" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="G62" s="55" t="s">
+      <c r="G71" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H62" s="57" t="s">
+      <c r="H71" s="44" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="49" t="s">
+    <row r="72" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B63" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="24" t="s">
+      <c r="B72" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D72" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E63" s="24"/>
-      <c r="G63" s="1" t="str">
-        <f t="shared" ref="G63:G73" si="0">_xlfn.CONCAT("AS_", _xlfn.TEXTJOIN("_", TRUE, B63:E63))</f>
+      <c r="E72" s="24"/>
+      <c r="G72" s="1" t="str">
+        <f t="shared" ref="G72:G82" si="0">_xlfn.CONCAT("AS_", _xlfn.TEXTJOIN("_", TRUE, B72:E72))</f>
         <v>AS_UnArmed_Standing_Looking_Up</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A64" s="44"/>
-      <c r="B64" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="24" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A73" s="24"/>
+      <c r="B73" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D73" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E64" s="24"/>
-      <c r="G64" s="1" t="str">
+      <c r="E73" s="24"/>
+      <c r="G73" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AS_UnArmed_Standing_Looking_Down</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A65" s="44"/>
-      <c r="B65" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="24" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A74" s="24"/>
+      <c r="B74" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="24" t="s">
+      <c r="D74" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E65" s="24"/>
-      <c r="G65" s="1" t="str">
+      <c r="E74" s="24"/>
+      <c r="G74" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AS_UnArmed_Standing_Looking_Left</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A66" s="44"/>
-      <c r="B66" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="24" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A75" s="24"/>
+      <c r="B75" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="24" t="s">
+      <c r="D75" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E66" s="24"/>
-      <c r="G66" s="1" t="str">
+      <c r="E75" s="24"/>
+      <c r="G75" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AS_UnArmed_Standing_Looking_Right</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B67" s="48"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B68" s="48"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A69" s="51"/>
-      <c r="B69" s="45"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A70" s="52" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B76" s="35"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B77" s="35"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A78" s="38"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A79" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="B79" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C79" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24" t="s">
+      <c r="D79" s="24"/>
+      <c r="E79" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G70" s="1" t="str">
-        <f t="shared" ref="G70" si="1">_xlfn.CONCAT("AS_", _xlfn.TEXTJOIN("_", TRUE, B70:E70))</f>
+      <c r="G79" s="1" t="str">
+        <f t="shared" ref="G79" si="1">_xlfn.CONCAT("AS_", _xlfn.TEXTJOIN("_", TRUE, B79:E79))</f>
         <v>AS_Rifle_Standing_Obstructed</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A71" s="52" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A80" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="45" t="s">
+      <c r="B80" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C80" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24" t="s">
+      <c r="D80" s="24"/>
+      <c r="E80" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="G71" s="1" t="str">
+      <c r="G80" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AS_Rifle_Standing_Low</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A72" s="52" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A81" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="45" t="s">
+      <c r="B81" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C81" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E72" s="24" t="s">
+      <c r="E81" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G72" s="1" t="str">
+      <c r="G81" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AS_Rifle_Standing_Hip</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A73" s="52" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A82" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="45" t="s">
+      <c r="B82" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C82" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E73" s="24" t="s">
+      <c r="E82" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G73" s="1" t="str">
+      <c r="G82" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AS_Rifle_Standing_Idle</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B77" s="35" t="s">
+    <row r="86" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B86" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="35"/>
-    </row>
-    <row r="78" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="28" t="s">
+      <c r="C86" s="51"/>
+      <c r="D86" s="51"/>
+      <c r="E86" s="51"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="51"/>
+    </row>
+    <row r="87" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C87" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D87" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="F87" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="G87" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H78" s="4" t="s">
+      <c r="H87" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="24" t="s">
+    <row r="88" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B79" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79" s="24" t="s">
+      <c r="B88" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D79" s="24" t="s">
+      <c r="D88" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E88" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="G79" s="1" t="str">
-        <f>_xlfn.CONCAT("AS_", _xlfn.TEXTJOIN("_", TRUE, B79:E79))</f>
+      <c r="G88" s="1" t="str">
+        <f>_xlfn.CONCAT("AS_", _xlfn.TEXTJOIN("_", TRUE, B88:E88))</f>
         <v>AS_UnArmed_Standing_Looking_Up</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B83" s="10" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B92" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B84" s="11" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B93" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B85" s="12"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B86" s="10" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B94" s="12"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B95" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B87" s="11" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B96" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B88" s="12"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B89" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B90" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B91" s="12"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B92" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B93" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B94" s="12"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B95" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B96" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B97" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="B97" s="12"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B98" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B99" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B100" s="12"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B101" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B102" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B103" s="12"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B104" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B105" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B106" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B107" s="10" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="B86:H86"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A61:H61"/>
+    <mergeCell ref="A70:H70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D16:D24" xr:uid="{8A2048BB-0B0E-481C-A99A-8807A38FC692}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D15 D25:D33" xr:uid="{8A2048BB-0B0E-481C-A99A-8807A38FC692}">
       <formula1>"-, Running, Walking"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B25 B53" xr:uid="{107A51C1-2430-44E8-84D9-1EB51726B5C2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62 B4:B6 B8:B34" xr:uid="{107A51C1-2430-44E8-84D9-1EB51726B5C2}">
       <formula1>"UnArmed, Rifle"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C25" xr:uid="{6EC3B352-1008-48AB-B172-162FB7B687BD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C34" xr:uid="{6EC3B352-1008-48AB-B172-162FB7B687BD}">
       <formula1>"Standing, Crouching, Pruning"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D53" xr:uid="{0A983BD9-AA13-42B1-9748-0CCEF3AA15DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34 D62" xr:uid="{0A983BD9-AA13-42B1-9748-0CCEF3AA15DB}">
       <formula1>"-, Running, Walking, Sprinting"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3840,17 +4000,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -3943,30 +4103,30 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="15" spans="1:10" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
@@ -5007,17 +5167,17 @@
       <c r="J61" s="2"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B62" s="35" t="s">
+      <c r="B62" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B63" s="4" t="s">
@@ -5165,17 +5325,17 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="35"/>
-      <c r="I75" s="35"/>
-      <c r="J75" s="35"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="51"/>
+      <c r="E75" s="51"/>
+      <c r="F75" s="51"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="51"/>
+      <c r="J75" s="51"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B76" s="4" t="s">

</xml_diff>